<commit_message>
updated with full values and formatting
</commit_message>
<xml_diff>
--- a/example_input_file.xlsx
+++ b/example_input_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barrapeak/Dropbox/Code/GitHub/polished-ZHe-derived-values/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC95EE65-80DD-9A4D-87D8-C5D5FAF6AE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B44291-132F-DF44-AE07-77225B39C519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2040" windowWidth="27640" windowHeight="16440" xr2:uid="{C19AACAB-A493-6A4A-9443-F0F7942C5B43}"/>
+    <workbookView xWindow="1160" yWindow="1560" windowWidth="27640" windowHeight="16440" xr2:uid="{C19AACAB-A493-6A4A-9443-F0F7942C5B43}"/>
   </bookViews>
   <sheets>
     <sheet name="example_input_data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Ellipse1_5">#REF!</definedName>
     <definedName name="gauss">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Crystal Fragment?</t>
   </si>
@@ -59,21 +59,9 @@
     <t>(ng)</t>
   </si>
   <si>
-    <t>z005</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>z007</t>
-  </si>
-  <si>
-    <t>z021</t>
-  </si>
-  <si>
     <t>References cited in footnotes</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
   </si>
   <si>
     <t>Ketcham, R.A., Gautheron, C., and Tassan-Got, L., 2011, Accounting for long alpha-particle stopping distances in (U-Th-Sm)/He geochronology: Refinement of the baseline case: Geochimica et Cosmochimica Acta, v. 75, p. 7779–7791, doi: 10.1016/j.gca.2011.10.011.</t>
-  </si>
-  <si>
-    <t>Laser Session</t>
   </si>
   <si>
     <t>Grain</t>
@@ -171,18 +156,9 @@
     </r>
   </si>
   <si>
-    <t>Grain - Zircon grain analyzed.</t>
-  </si>
-  <si>
-    <t>Laser Session - U-Pb LA-ICP-MS data collection session if applicable.</t>
-  </si>
-  <si>
     <t>Length - Length is measured parallel to the c-axis and includes pyramidal terminations for tetragonal grians. It is measured twice on two perpendicular sides.</t>
   </si>
   <si>
-    <t>Width - Width 1 is measured perpendicular to the c-axis. Width 2 is measured perpendicular to both the c-axis and Width 1.</t>
-  </si>
-  <si>
     <t>Length Polished Face - the long axis of the polished face of the grain. Only needed for ellipsoid grains polished less than halfway. Enter zero if not applicable.</t>
   </si>
   <si>
@@ -202,7 +178,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">4He - Blank-corrected </t>
+      <t xml:space="preserve">Uncertainties on </t>
     </r>
     <r>
       <rPr>
@@ -221,12 +197,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>He measurement.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Uncertainties on </t>
+      <t>He, U, Th, and Sm are reported as the 1σ standard deviation and include the propagated uncertainties on the measurements of the sample, blank, spike, and standard.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U - Total blank-corrected ng of </t>
     </r>
     <r>
       <rPr>
@@ -235,7 +211,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>4</t>
+      <t>238</t>
     </r>
     <r>
       <rPr>
@@ -245,12 +221,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>He, U, Th, and Sm are reported as the 1σ standard deviation and include the propagated uncertainties on the measurements of the sample, blank, spike, and standard.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">U - Total blank-corrected ng of </t>
+      <t xml:space="preserve">U and </t>
     </r>
     <r>
       <rPr>
@@ -259,7 +230,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>238</t>
+      <t>235</t>
     </r>
     <r>
       <rPr>
@@ -269,7 +240,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">U and </t>
+      <t xml:space="preserve">U. Total </t>
     </r>
     <r>
       <rPr>
@@ -278,7 +249,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>235</t>
+      <t>238</t>
     </r>
     <r>
       <rPr>
@@ -288,7 +259,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">U. Total </t>
+      <t xml:space="preserve">U is measured and </t>
     </r>
     <r>
       <rPr>
@@ -297,7 +268,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>238</t>
+      <t>235</t>
     </r>
     <r>
       <rPr>
@@ -307,7 +278,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">U is measured and </t>
+      <t xml:space="preserve">U is calculated assuming </t>
     </r>
     <r>
       <rPr>
@@ -326,7 +297,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">U is calculated assuming </t>
+      <t xml:space="preserve">U = </t>
     </r>
     <r>
       <rPr>
@@ -335,7 +306,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>235</t>
+      <t>238</t>
     </r>
     <r>
       <rPr>
@@ -345,7 +316,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">U = </t>
+      <t>U/137.818 after Hiess et al. (2012).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Th - Total blank-corrected ng of </t>
     </r>
     <r>
       <rPr>
@@ -354,7 +330,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>238</t>
+      <t>232</t>
     </r>
     <r>
       <rPr>
@@ -364,12 +340,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>U/137.818 after Hiess et al. (2012).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Th - Total blank-corrected ng of </t>
+      <t>Th</t>
+    </r>
+  </si>
+  <si>
+    <t>Length P</t>
+  </si>
+  <si>
+    <t>Width P</t>
+  </si>
+  <si>
+    <t>Table does not have to have footnotes, the script will remove them before calculating values.</t>
+  </si>
+  <si>
+    <t>The column headers listed are required. The code can accommodate extra columns as long as the required columns are present.</t>
+  </si>
+  <si>
+    <t>Analysis Session</t>
+  </si>
+  <si>
+    <t>Analysis Session - Internal ID for analysis reference, e.g., U-Pb LA-ICP-MS data collection session, U-Th-Sm solution ICP-MS data collection session, etc. If not applicable, fill column with 1.</t>
+  </si>
+  <si>
+    <t>Grain - Zircon grain analyzed. Can be a string of any length</t>
+  </si>
+  <si>
+    <t>Width - Width is measured perpendicular to the c-axis. Width 2 is measured perpendicular to both the c-axis and Width 1.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4He - Blank-corrected </t>
     </r>
     <r>
       <rPr>
@@ -378,7 +378,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>232</t>
+      <t>4</t>
     </r>
     <r>
       <rPr>
@@ -388,7 +388,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Th</t>
+      <t>He measurement in fmol. This is not used in the script but is required input for HeCalc or other date calculating programs.</t>
     </r>
   </si>
   <si>
@@ -412,23 +412,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Sm. In some cases Sm may not be measured, for example in minerals like zircon with negligible Sm. n.m. indicates when Sm is not measured.</t>
-    </r>
-  </si>
-  <si>
-    <t>Length P</t>
-  </si>
-  <si>
-    <t>Width P</t>
-  </si>
-  <si>
-    <t>Example Input Template</t>
-  </si>
-  <si>
-    <t>Table does not have to have footnotes, the script will remove them before calculating values.</t>
-  </si>
-  <si>
-    <t>The column headers listed are required. The code can accommodate extra columns as long as the required columns are present.</t>
+      <t>Sm.</t>
+    </r>
+  </si>
+  <si>
+    <t>z007a</t>
+  </si>
+  <si>
+    <t>z010b</t>
+  </si>
+  <si>
+    <t>z021e</t>
+  </si>
+  <si>
+    <t>Example Input Template - Example data is synthetic.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Crystal Fragment? - Whether or not the crystal is an interior fragment (no alpha-ejection rim present). Yes or No.</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -568,22 +571,12 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,11 +911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5D7F04-0E95-4F4F-886B-528A0899B539}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -942,72 +935,72 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1058,11 +1051,11 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5">
         <v>150</v>
@@ -1077,7 +1070,7 @@
         <v>63</v>
       </c>
       <c r="G4" s="6">
-        <v>88.09</v>
+        <v>90</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -1085,41 +1078,41 @@
       <c r="I4" s="5">
         <v>3</v>
       </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
+      <c r="J4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="7">
-        <v>2329.96</v>
-      </c>
-      <c r="O4" s="5">
-        <v>6.9</v>
+        <v>4</v>
+      </c>
+      <c r="N4" s="6">
+        <v>4350</v>
+      </c>
+      <c r="O4" s="6">
+        <v>12.882195402496182</v>
       </c>
       <c r="P4" s="8">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="Q4" s="5">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>1.2591133004926109E-2</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.624</v>
+      </c>
+      <c r="S4" s="8">
+        <v>1.027764705882353E-2</v>
+      </c>
+      <c r="T4" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R4" s="8">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="S4" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="T4" s="16">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="U4" s="16">
-        <v>1E-3</v>
+      <c r="U4" s="8">
+        <v>1.3333333333333333E-3</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1127,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5">
         <v>133</v>
@@ -1139,10 +1132,10 @@
         <v>132</v>
       </c>
       <c r="F5" s="5">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="G5" s="6">
-        <v>88.09</v>
+        <v>78</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
@@ -1151,40 +1144,40 @@
         <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K5" s="5">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L5" s="5">
         <v>0</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N5" s="7">
-        <v>1196.27</v>
-      </c>
-      <c r="O5" s="5">
-        <v>4.2</v>
+        <v>1196.5</v>
+      </c>
+      <c r="O5" s="7">
+        <v>4.2008075100102822</v>
       </c>
       <c r="P5" s="8">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>4.0000000000000001E-3</v>
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>5.061946902654867E-3</v>
       </c>
       <c r="R5" s="8">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="S5" s="5">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="T5" s="16">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="U5" s="16">
-        <v>8.0000000000000002E-3</v>
+        <v>0.22</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1.5648535564853558E-2</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="U5" s="8">
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1192,10 +1185,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="D6" s="5">
         <v>132</v>
@@ -1207,7 +1200,7 @@
         <v>129</v>
       </c>
       <c r="G6" s="6">
-        <v>88.09</v>
+        <v>100</v>
       </c>
       <c r="H6" s="5">
         <v>2</v>
@@ -1215,46 +1208,46 @@
       <c r="I6" s="5">
         <v>2</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
+      <c r="J6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="L6" s="5">
         <v>0</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N6" s="6">
-        <v>9504.3700000000008</v>
-      </c>
-      <c r="O6" s="5">
-        <v>19</v>
+        <v>6502.37</v>
+      </c>
+      <c r="O6" s="6">
+        <v>12.998760570137737</v>
       </c>
       <c r="P6" s="8">
-        <v>1.58</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>5.5E-2</v>
+        <v>2.0579999999999998</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>7.163924050632911E-2</v>
       </c>
       <c r="R6" s="8">
-        <v>2.04</v>
-      </c>
-      <c r="S6" s="5">
-        <v>2.7E-2</v>
-      </c>
-      <c r="T6" s="16">
+        <v>2</v>
+      </c>
+      <c r="S6" s="8">
+        <v>2.6470588235294117E-2</v>
+      </c>
+      <c r="T6" s="5">
         <v>0</v>
       </c>
-      <c r="U6" s="16">
+      <c r="U6" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1277,150 +1270,155 @@
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
     </row>
-    <row r="8" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-    </row>
-    <row r="9" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="22" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="22" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="22" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="22" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="22" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="22" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-    </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>10</v>
+      <c r="A27" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>